<commit_message>
FEAT : finish parsing Utility
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="parse" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="CAPCOST" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="UTILITY" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1115,22 +1116,22 @@
         <v>2.2628</v>
       </c>
       <c r="I2" t="n">
-        <v>4.3247</v>
+        <v>2.2891</v>
       </c>
       <c r="J2" t="n">
-        <v>4.3247</v>
+        <v>2.2891</v>
       </c>
       <c r="K2" t="n">
         <v>2.2628</v>
       </c>
       <c r="L2" t="n">
-        <v>4.3247</v>
+        <v>2.2891</v>
       </c>
       <c r="M2" t="n">
         <v>2.2628</v>
       </c>
       <c r="N2" t="n">
-        <v>4.3247</v>
+        <v>2.2891</v>
       </c>
       <c r="O2" t="n">
         <v>2.2628</v>
@@ -1139,7 +1140,7 @@
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="n">
-        <v>4.3247</v>
+        <v>2.2891</v>
       </c>
     </row>
     <row r="3">
@@ -1166,22 +1167,22 @@
         <v>0.8581</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.303</v>
+        <v>1.3604</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.303</v>
+        <v>1.3604</v>
       </c>
       <c r="K3" t="n">
         <v>0.8581</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.303</v>
+        <v>1.3604</v>
       </c>
       <c r="M3" t="n">
         <v>0.8581</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.303</v>
+        <v>1.3604</v>
       </c>
       <c r="O3" t="n">
         <v>0.8581</v>
@@ -1190,7 +1191,7 @@
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="n">
-        <v>-0.303</v>
+        <v>1.3604</v>
       </c>
     </row>
     <row r="4">
@@ -1217,22 +1218,22 @@
         <v>0.0003</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1634</v>
+        <v>-0.1027</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1634</v>
+        <v>-0.1027</v>
       </c>
       <c r="K4" t="n">
         <v>0.0003</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1634</v>
+        <v>-0.1027</v>
       </c>
       <c r="M4" t="n">
         <v>0.0003</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1634</v>
+        <v>-0.1027</v>
       </c>
       <c r="O4" t="n">
         <v>0.0003</v>
@@ -1241,7 +1242,7 @@
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="n">
-        <v>0.1634</v>
+        <v>-0.1027</v>
       </c>
     </row>
     <row r="5">
@@ -1375,7 +1376,7 @@
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
-        <v>128000</v>
+        <v>1837738.887525055</v>
       </c>
       <c r="D8" t="n">
         <v>73836.96864644403</v>
@@ -1388,36 +1389,34 @@
         <v>147875.0306900121</v>
       </c>
       <c r="H8" t="n">
-        <v>53900</v>
+        <v>1976709.767700679</v>
       </c>
       <c r="I8" t="n">
-        <v>3124700</v>
+        <v>1481215.826683687</v>
       </c>
       <c r="J8" t="n">
-        <v>3690800</v>
+        <v>994189.8037161557</v>
       </c>
       <c r="K8" t="n">
         <v>69206.92483863865</v>
       </c>
       <c r="L8" t="n">
-        <v>2858200</v>
+        <v>1221426.706326984</v>
       </c>
       <c r="M8" t="n">
-        <v>377000</v>
+        <v>4232444.44902235</v>
       </c>
       <c r="N8" t="n">
-        <v>242936036229094.2</v>
+        <v>1416467.388385196</v>
       </c>
       <c r="O8" t="n">
-        <v>25500</v>
+        <v>1470768.43577163</v>
       </c>
       <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="n">
-        <v>336000</v>
-      </c>
+      <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="n">
-        <v>2072700</v>
+        <v>640555.8597020187</v>
       </c>
     </row>
     <row r="9">
@@ -1464,4 +1463,243 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>H-COMP-1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>H-COMP-2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>H-HTX-1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>HTX-02</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>HTX-03</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>HTX-04</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>HTX-05</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>N-COMP-1</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>N-COMP-2</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>N-COMP-3</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>N-HTX-1</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>N-HTX-2</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>NH3FLASH</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>REACT-1</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>REACT-2</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>REACT-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ELECTRICITY UTILITY</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ELECTRICITY UTILITY</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>COOLING UTILITY</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>HOT UTILITY</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>ELECTRICITY UTILITY</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>COOLING UTILITY</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>ELECTRICITY UTILITY</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>ELECTRICITY UTILITY</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>ELECTRICITY UTILITY</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>ELECTRICITY UTILITY</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>COOLING UTILITY</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>COOLING UTILITY</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>HOT UTILITY</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>HOT UTILITY</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>HOT UTILITY</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>HOT UTILITY</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>4153.8584</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3865.109</v>
+      </c>
+      <c r="D3" t="n">
+        <v>609760</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1348.87976</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1070.8652</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2168900</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2284.7394</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2238.2037</v>
+      </c>
+      <c r="J3" t="n">
+        <v>3059.7322</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1194.7998</v>
+      </c>
+      <c r="L3" t="n">
+        <v>372530</v>
+      </c>
+      <c r="M3" t="n">
+        <v>540000</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-70.37069600000001</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-8882.631999999998</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-5950.903200000001</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-3961.578560000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>